<commit_message>
hr_boot: pogress button and adding data
</commit_message>
<xml_diff>
--- a/hr_bot/V2/sas_20_01_17 Example Jobpost Website1.xlsx
+++ b/hr_bot/V2/sas_20_01_17 Example Jobpost Website1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.seebacher\Desktop\PeakAce\_SAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.bakhabou\Documents\repositories_peak_ace\hr_bot\V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5053E85C-9F35-488C-B15A-35760CF7E8B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F14CE9-1ABF-4D72-AE0F-CEDC030A2D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4EF943A2-2CD1-48F2-81ED-629C0E7E8563}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
   <si>
     <t>JOB</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Veröffentlichen bis</t>
   </si>
   <si>
-    <t xml:space="preserve">filled automatically </t>
-  </si>
-  <si>
     <t>Community-Management</t>
   </si>
   <si>
@@ -319,12 +316,6 @@
   </si>
   <si>
     <t xml:space="preserve">tick both boxes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">keep it empty </t>
-  </si>
-  <si>
-    <t>keep it empty</t>
   </si>
   <si>
     <t>Job-Titel / Position</t>
@@ -558,9 +549,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -576,7 +567,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -876,10 +867,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -1021,9 +1012,7 @@
       <c r="F3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="G3" s="7"/>
       <c r="H3">
         <v>10999</v>
       </c>
@@ -1039,29 +1028,25 @@
       <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>86</v>
-      </c>
+      <c r="N3" s="7"/>
       <c r="O3" s="6" t="s">
         <v>43</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="Q3" s="7"/>
       <c r="R3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1119,7 +1104,7 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -1149,10 +1134,10 @@
         <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1163,10 +1148,10 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1177,10 +1162,10 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1191,132 +1176,132 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1317,7 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
@@ -1356,114 +1341,114 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="M2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="P2" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" t="s">
         <v>109</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="E3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>43</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K3" t="s">
         <v>37</v>
@@ -1472,13 +1457,13 @@
         <v>38</v>
       </c>
       <c r="M3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hr_boot: adding the rockitBerlin platform
</commit_message>
<xml_diff>
--- a/hr_bot/V2/sas_20_01_17 Example Jobpost Website1.xlsx
+++ b/hr_bot/V2/sas_20_01_17 Example Jobpost Website1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.bakhabou\Documents\repositories_peak_ace\hr_bot\V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F14CE9-1ABF-4D72-AE0F-CEDC030A2D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CB890E-2C46-4484-B40A-E740290A1451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4EF943A2-2CD1-48F2-81ED-629C0E7E8563}"/>
+    <workbookView xWindow="8700" yWindow="1185" windowWidth="16755" windowHeight="11385" activeTab="2" xr2:uid="{4EF943A2-2CD1-48F2-81ED-629C0E7E8563}"/>
   </bookViews>
   <sheets>
     <sheet name="Creative City" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
   <si>
     <t>JOB</t>
   </si>
@@ -423,12 +423,6 @@
     <t>nothing</t>
   </si>
   <si>
-    <t>Keine + Erste</t>
-  </si>
-  <si>
-    <t>Marketing/ Online Marketing &amp; Suchmaschinenmarketing (SEM/ SEA)</t>
-  </si>
-  <si>
     <t>https://www.pa.ag/de/job/sea-junior-manager-m-w-d/?utm_medium=organic&amp;utm_source=rockitdigital&amp;utm_campaign=jobs&amp;utm_content=sea_junior_manager_mwd</t>
   </si>
   <si>
@@ -442,6 +436,12 @@
   </si>
   <si>
     <t>www.pa.ag/de/job</t>
+  </si>
+  <si>
+    <t>Keine , Erste</t>
+  </si>
+  <si>
+    <t>Marketing/ Online Marketing , Suchmaschinenmarketing (SEM/ SEA)</t>
   </si>
 </sst>
 </file>
@@ -865,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF6B204-FFF1-4849-9775-4765AF1CF192}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
@@ -1313,18 +1313,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEC6FF-5A3B-4D72-BA10-58B0D3FFA9C7}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="63.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.7109375" bestFit="1" customWidth="1"/>
@@ -1429,26 +1429,24 @@
       <c r="C3" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>108</v>
-      </c>
+      <c r="D3" s="7"/>
       <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>43</v>
       </c>
       <c r="I3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K3" t="s">
         <v>37</v>
@@ -1457,10 +1455,10 @@
         <v>38</v>
       </c>
       <c r="M3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O3" s="7" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
hr_boot: trying with Iframe data
</commit_message>
<xml_diff>
--- a/hr_bot/V2/sas_20_01_17 Example Jobpost Website1.xlsx
+++ b/hr_bot/V2/sas_20_01_17 Example Jobpost Website1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.bakhabou\Documents\repositories_peak_ace\hr_bot\V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CB890E-2C46-4484-B40A-E740290A1451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D282EA2-4FE1-46E7-A16A-F0CF2CBC1EB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8700" yWindow="1185" windowWidth="16755" windowHeight="11385" activeTab="2" xr2:uid="{4EF943A2-2CD1-48F2-81ED-629C0E7E8563}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="116">
   <si>
     <t>JOB</t>
   </si>
@@ -863,11 +863,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF6B204-FFF1-4849-9775-4765AF1CF192}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,6 +1049,62 @@
         <v>83</v>
       </c>
     </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4">
+        <v>10999</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" t="s">
+        <v>81</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
@@ -1060,35 +1116,37 @@
   <hyperlinks>
     <hyperlink ref="O3" r:id="rId1" xr:uid="{9632FA7E-5EB7-4BF7-A2FF-5CDC53B420AD}"/>
     <hyperlink ref="P3" r:id="rId2" xr:uid="{F494BAC3-00B3-4F0D-993F-35F39DB92692}"/>
+    <hyperlink ref="O4" r:id="rId3" xr:uid="{2A74F0D6-ABB4-42FE-85A2-3CE724DC3237}"/>
+    <hyperlink ref="P4" r:id="rId4" xr:uid="{B7748269-168C-407C-8A4F-D23EC17E8FD8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3EEB3A78-F033-4D8D-8839-BA07FEFD2733}">
           <x14:formula1>
             <xm:f>enums!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
+          <xm:sqref>B3:B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C5DC8DA0-7D9A-413B-949B-8E731005DEFC}">
           <x14:formula1>
             <xm:f>enums!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
+          <xm:sqref>C3:C4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DB0B0DCD-3E6D-4C6A-8A94-46F6E4B669E2}">
           <x14:formula1>
             <xm:f>enums!$E$2:$E$24</xm:f>
           </x14:formula1>
-          <xm:sqref>R3</xm:sqref>
+          <xm:sqref>R3:R4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7114FD69-0D83-418B-B7DC-E64F2FE5D5A3}">
           <x14:formula1>
             <xm:f>enums!$G$2:$G$14</xm:f>
           </x14:formula1>
-          <xm:sqref>T3</xm:sqref>
+          <xm:sqref>T3:T4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1311,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEC6FF-5A3B-4D72-BA10-58B0D3FFA9C7}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,6 +1522,14 @@
         <v>108</v>
       </c>
     </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="D4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>

</xml_diff>

<commit_message>
hr_bot: manipulating the frame and injecting js into it
</commit_message>
<xml_diff>
--- a/hr_bot/V2/sas_20_01_17 Example Jobpost Website1.xlsx
+++ b/hr_bot/V2/sas_20_01_17 Example Jobpost Website1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.bakhabou\Documents\repositories_peak_ace\hr_bot\V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D282EA2-4FE1-46E7-A16A-F0CF2CBC1EB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD9CBC4-75F3-4265-9FA8-78D14AD4A451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="1185" windowWidth="16755" windowHeight="11385" activeTab="2" xr2:uid="{4EF943A2-2CD1-48F2-81ED-629C0E7E8563}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4EF943A2-2CD1-48F2-81ED-629C0E7E8563}"/>
   </bookViews>
   <sheets>
     <sheet name="Creative City" sheetId="1" r:id="rId1"/>
@@ -1372,7 +1372,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>